<commit_message>
Fixed version of HW1
</commit_message>
<xml_diff>
--- a/hw1.xlsx
+++ b/hw1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Desktop\cheme375B\hw1-JeremyRHook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35BDFEC3-11D4-4642-BC59-3A1E29A2F243}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C244AB-2E9D-4133-9D18-29C06EE8A706}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="204" windowWidth="11748" windowHeight="10092" firstSheet="3" activeTab="5" xr2:uid="{C1BFDA8D-4032-4EE1-9A35-B763494A400C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{C1BFDA8D-4032-4EE1-9A35-B763494A400C}"/>
   </bookViews>
   <sheets>
     <sheet name="HW1_P1" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -97,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="111">
   <si>
     <t>Thermal Conductivity (k)</t>
   </si>
@@ -419,6 +421,18 @@
   <si>
     <t>Moles</t>
   </si>
+  <si>
+    <t>Pressures (atm)</t>
+  </si>
+  <si>
+    <t>Temperature Table (K)</t>
+  </si>
+  <si>
+    <t>Acceptable Temperature ranges are 119.26-596.3 Degrees Kelvin</t>
+  </si>
+  <si>
+    <t>For varrying Pressures and Volumes</t>
+  </si>
 </sst>
 </file>
 
@@ -427,7 +441,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,6 +537,23 @@
       <color rgb="FF24292E"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="22">
@@ -689,7 +720,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -792,6 +823,10 @@
     <xf numFmtId="0" fontId="13" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -903,9 +938,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -914,38 +948,17 @@
             <c:v>High</c:v>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$G$4:$G$33</c:f>
@@ -1045,6 +1058,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E9E0-4B73-B200-5AD5E47FBDBE}"/>
@@ -1058,38 +1072,17 @@
             <c:v>Low</c:v>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent4">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent4">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$H$4:$H$33</c:f>
@@ -1189,6 +1182,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-E9E0-4B73-B200-5AD5E47FBDBE}"/>
@@ -1202,38 +1196,17 @@
             <c:v>Close</c:v>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent6">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent6">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$I$4:$I$33</c:f>
@@ -1333,6 +1306,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-E9E0-4B73-B200-5AD5E47FBDBE}"/>
@@ -1347,11 +1321,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="100"/>
-        <c:overlap val="-24"/>
+        <c:smooth val="0"/>
         <c:axId val="396512288"/>
         <c:axId val="396511632"/>
-      </c:barChart>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="396512288"/>
         <c:scaling>
@@ -2544,9 +2517,8 @@
           <c:h val="0.83976818238769224"/>
         </c:manualLayout>
       </c:layout>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -2555,15 +2527,17 @@
             <c:v>NFLX HIGH</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$O$72:$O$101</c:f>
@@ -2663,6 +2637,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6F96-4081-8062-827094A249E9}"/>
@@ -2676,15 +2651,17 @@
             <c:v>NFLX LOW</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$P$72:$P$101</c:f>
@@ -2784,6 +2761,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6F96-4081-8062-827094A249E9}"/>
@@ -2797,15 +2775,17 @@
             <c:v>NFLX CLOSE</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$Q$72:$Q$101</c:f>
@@ -2905,6 +2885,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-6F96-4081-8062-827094A249E9}"/>
@@ -2918,15 +2899,17 @@
             <c:v>SBUX HIGH</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$R$72:$R$101</c:f>
@@ -3026,6 +3009,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-6F96-4081-8062-827094A249E9}"/>
@@ -3039,15 +3023,17 @@
             <c:v>SBUX LOW</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$S$72:$S$101</c:f>
@@ -3147,6 +3133,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-6F96-4081-8062-827094A249E9}"/>
@@ -3160,15 +3147,17 @@
             <c:v>SBUX CLOSE</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$T$72:$T$101</c:f>
@@ -3268,6 +3257,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-6F96-4081-8062-827094A249E9}"/>
@@ -3282,10 +3272,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:smooth val="0"/>
         <c:axId val="542691920"/>
         <c:axId val="542695200"/>
-      </c:barChart>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="542691920"/>
         <c:scaling>
@@ -3528,8 +3518,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.96322229051286212"/>
           <c:y val="0.24151272714986663"/>
-          <c:w val="3.6777709487137829E-2"/>
-          <c:h val="0.37586202439321864"/>
+          <c:w val="3.6777709831509381E-2"/>
+          <c:h val="9.245910706213302E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3686,9 +3676,8 @@
           <c:h val="0.83553112110367456"/>
         </c:manualLayout>
       </c:layout>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -3697,38 +3686,17 @@
             <c:v>HIGH</c:v>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent6">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent6">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$G$38:$G$67</c:f>
@@ -3828,6 +3796,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8A64-4072-AC7D-B2C1ADD6D67D}"/>
@@ -3841,38 +3810,17 @@
             <c:v>LOW</c:v>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent5">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent5">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$H$38:$H$67</c:f>
@@ -3972,6 +3920,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8A64-4072-AC7D-B2C1ADD6D67D}"/>
@@ -3985,38 +3934,17 @@
             <c:v>CLOSE</c:v>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent4">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent4">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$I$38:$I$67</c:f>
@@ -4116,6 +4044,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-8A64-4072-AC7D-B2C1ADD6D67D}"/>
@@ -4130,10 +4059,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:smooth val="0"/>
         <c:axId val="396259712"/>
         <c:axId val="396261024"/>
-      </c:barChart>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="396259712"/>
         <c:scaling>
@@ -4517,9 +4446,8 @@
           <c:h val="0.83976818238769224"/>
         </c:manualLayout>
       </c:layout>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -4528,15 +4456,17 @@
             <c:v>NFLX HIGH</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$O$72:$O$101</c:f>
@@ -4636,6 +4566,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3BDD-44D4-A718-F167A94E43F4}"/>
@@ -4649,15 +4580,17 @@
             <c:v>NFLX LOW</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$P$72:$P$101</c:f>
@@ -4757,6 +4690,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3BDD-44D4-A718-F167A94E43F4}"/>
@@ -4770,15 +4704,17 @@
             <c:v>NFLX CLOSE</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$Q$72:$Q$101</c:f>
@@ -4878,6 +4814,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-3BDD-44D4-A718-F167A94E43F4}"/>
@@ -4891,15 +4828,17 @@
             <c:v>SBUX HIGH</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$R$72:$R$101</c:f>
@@ -4999,6 +4938,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-3BDD-44D4-A718-F167A94E43F4}"/>
@@ -5012,15 +4952,17 @@
             <c:v>SBUX LOW</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$S$72:$S$101</c:f>
@@ -5120,6 +5062,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-3BDD-44D4-A718-F167A94E43F4}"/>
@@ -5133,15 +5076,17 @@
             <c:v>SBUX CLOSE</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>'HW1_P3(A)'!$T$72:$T$101</c:f>
@@ -5241,6 +5186,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-3BDD-44D4-A718-F167A94E43F4}"/>
@@ -5255,10 +5201,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:smooth val="0"/>
         <c:axId val="542691920"/>
         <c:axId val="542695200"/>
-      </c:barChart>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="542691920"/>
         <c:scaling>
@@ -5501,8 +5447,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.96322229051286212"/>
           <c:y val="0.24151272714986663"/>
-          <c:w val="3.6777709487137829E-2"/>
-          <c:h val="0.37586202439321864"/>
+          <c:w val="3.6777733208596064E-2"/>
+          <c:h val="0.16618370823676104"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -22248,10 +22194,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>554182</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>115453</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>219364</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>46180</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="7273636" cy="1125693"/>
     <xdr:sp macro="" textlink="">
@@ -22267,7 +22213,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="554182" y="6026726"/>
+          <a:off x="9132455" y="600362"/>
           <a:ext cx="7273636" cy="1125693"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -23253,17 +23199,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8278783-BE3B-4621-80A5-CAFE19EF61F4}">
-  <dimension ref="A1:V32"/>
+  <dimension ref="A1:V54"/>
   <sheetViews>
-    <sheetView zoomScale="66" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="66" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="AB31" sqref="AB31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
-    <col min="2" max="2" width="40.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" customWidth="1"/>
     <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.77734375" customWidth="1"/>
@@ -23566,7 +23512,7 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="A13" s="54">
         <f>A12+25</f>
         <v>125</v>
       </c>
@@ -23656,7 +23602,7 @@
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+      <c r="A14" s="54">
         <f t="shared" ref="A14:A32" si="20">A13+25</f>
         <v>150</v>
       </c>
@@ -23746,7 +23692,7 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+      <c r="A15" s="54">
         <f t="shared" si="20"/>
         <v>175</v>
       </c>
@@ -23836,7 +23782,7 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+      <c r="A16" s="54">
         <f t="shared" si="20"/>
         <v>200</v>
       </c>
@@ -23926,7 +23872,7 @@
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+      <c r="A17" s="54">
         <f t="shared" si="20"/>
         <v>225</v>
       </c>
@@ -24016,7 +23962,7 @@
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+      <c r="A18" s="54">
         <f t="shared" si="20"/>
         <v>250</v>
       </c>
@@ -24106,7 +24052,7 @@
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
+      <c r="A19" s="54">
         <f t="shared" si="20"/>
         <v>275</v>
       </c>
@@ -24196,7 +24142,7 @@
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+      <c r="A20" s="54">
         <f t="shared" si="20"/>
         <v>300</v>
       </c>
@@ -24286,7 +24232,7 @@
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
+      <c r="A21" s="54">
         <f t="shared" si="20"/>
         <v>325</v>
       </c>
@@ -24376,7 +24322,7 @@
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
+      <c r="A22" s="54">
         <f t="shared" si="20"/>
         <v>350</v>
       </c>
@@ -24466,7 +24412,7 @@
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+      <c r="A23" s="54">
         <f t="shared" si="20"/>
         <v>375</v>
       </c>
@@ -24556,7 +24502,7 @@
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+      <c r="A24" s="54">
         <f t="shared" si="20"/>
         <v>400</v>
       </c>
@@ -24646,7 +24592,7 @@
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
+      <c r="A25" s="54">
         <f t="shared" si="20"/>
         <v>425</v>
       </c>
@@ -24736,7 +24682,7 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
+      <c r="A26" s="54">
         <f t="shared" si="20"/>
         <v>450</v>
       </c>
@@ -24826,7 +24772,7 @@
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
+      <c r="A27" s="54">
         <f t="shared" si="20"/>
         <v>475</v>
       </c>
@@ -24916,7 +24862,7 @@
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
+      <c r="A28" s="54">
         <f t="shared" si="20"/>
         <v>500</v>
       </c>
@@ -25006,7 +24952,7 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A29" s="3">
+      <c r="A29" s="54">
         <f t="shared" si="20"/>
         <v>525</v>
       </c>
@@ -25096,7 +25042,7 @@
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
+      <c r="A30" s="54">
         <f t="shared" si="20"/>
         <v>550</v>
       </c>
@@ -25186,7 +25132,7 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A31" s="3">
+      <c r="A31" s="54">
         <f t="shared" si="20"/>
         <v>575</v>
       </c>
@@ -25363,6 +25309,1543 @@
       <c r="V32">
         <f t="shared" si="19"/>
         <v>2.515512326010398</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B34" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B35" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" s="4">
+        <f>500</f>
+        <v>500</v>
+      </c>
+      <c r="C38" s="4">
+        <f>B38+25</f>
+        <v>525</v>
+      </c>
+      <c r="D38" s="4">
+        <f t="shared" ref="D38" si="22">C38+25</f>
+        <v>550</v>
+      </c>
+      <c r="E38" s="4">
+        <f t="shared" ref="E38" si="23">D38+25</f>
+        <v>575</v>
+      </c>
+      <c r="F38" s="4">
+        <f t="shared" ref="F38" si="24">E38+25</f>
+        <v>600</v>
+      </c>
+      <c r="G38" s="4">
+        <f t="shared" ref="G38" si="25">F38+25</f>
+        <v>625</v>
+      </c>
+      <c r="H38" s="4">
+        <f t="shared" ref="H38" si="26">G38+25</f>
+        <v>650</v>
+      </c>
+      <c r="I38" s="4">
+        <f t="shared" ref="I38" si="27">H38+25</f>
+        <v>675</v>
+      </c>
+      <c r="J38" s="4">
+        <f t="shared" ref="J38" si="28">I38+25</f>
+        <v>700</v>
+      </c>
+      <c r="K38" s="4">
+        <f t="shared" ref="K38" si="29">J38+25</f>
+        <v>725</v>
+      </c>
+      <c r="L38" s="4">
+        <f t="shared" ref="L38" si="30">K38+25</f>
+        <v>750</v>
+      </c>
+      <c r="M38" s="4">
+        <f t="shared" ref="M38" si="31">L38+25</f>
+        <v>775</v>
+      </c>
+      <c r="N38" s="4">
+        <f t="shared" ref="N38" si="32">M38+25</f>
+        <v>800</v>
+      </c>
+      <c r="O38" s="4">
+        <f t="shared" ref="O38" si="33">N38+25</f>
+        <v>825</v>
+      </c>
+      <c r="P38" s="4">
+        <f t="shared" ref="P38" si="34">O38+25</f>
+        <v>850</v>
+      </c>
+      <c r="Q38" s="4">
+        <f t="shared" ref="Q38" si="35">P38+25</f>
+        <v>875</v>
+      </c>
+      <c r="R38" s="4">
+        <f t="shared" ref="R38" si="36">Q38+25</f>
+        <v>900</v>
+      </c>
+      <c r="S38" s="4">
+        <f t="shared" ref="S38" si="37">R38+25</f>
+        <v>925</v>
+      </c>
+      <c r="T38" s="4">
+        <f t="shared" ref="T38" si="38">S38+25</f>
+        <v>950</v>
+      </c>
+      <c r="U38" s="4">
+        <f>T38+25</f>
+        <v>975</v>
+      </c>
+      <c r="V38" s="4">
+        <f t="shared" ref="V38" si="39">U38+25</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A39" s="56">
+        <v>1</v>
+      </c>
+      <c r="B39" s="55">
+        <f t="shared" ref="B39:B54" si="40" xml:space="preserve"> A39*$B$38/(n1_N2*R_N2)</f>
+        <v>119.25999999999998</v>
+      </c>
+      <c r="C39" s="55">
+        <f t="shared" ref="C39:C54" si="41" xml:space="preserve"> A39*$C$38/(n1_N2*R_N2)</f>
+        <v>125.22299999999998</v>
+      </c>
+      <c r="D39" s="55">
+        <f t="shared" ref="D39:D54" si="42" xml:space="preserve"> A39*$D$38/(n1_N2*R_N2)</f>
+        <v>131.18599999999998</v>
+      </c>
+      <c r="E39" s="55">
+        <f t="shared" ref="E39:E54" si="43" xml:space="preserve"> A39*$E$38/(n1_N2*R_N2)</f>
+        <v>137.14899999999997</v>
+      </c>
+      <c r="F39" s="55">
+        <f t="shared" ref="F39:F54" si="44" xml:space="preserve"> A39*$F$38/(n1_N2*R_N2)</f>
+        <v>143.11199999999997</v>
+      </c>
+      <c r="G39" s="55">
+        <f t="shared" ref="G39:G54" si="45" xml:space="preserve"> A39*$G$38/(n1_N2*R_N2)</f>
+        <v>149.07499999999996</v>
+      </c>
+      <c r="H39" s="55">
+        <f t="shared" ref="H39:H54" si="46" xml:space="preserve"> A39*$H$38/(n1_N2*R_N2)</f>
+        <v>155.03799999999998</v>
+      </c>
+      <c r="I39" s="55">
+        <f t="shared" ref="I39:I54" si="47" xml:space="preserve"> A39*$I$38/(n1_N2*R_N2)</f>
+        <v>161.00099999999998</v>
+      </c>
+      <c r="J39" s="55">
+        <f t="shared" ref="J39:J54" si="48" xml:space="preserve"> A39*$J$38/(n1_N2*R_N2)</f>
+        <v>166.96399999999997</v>
+      </c>
+      <c r="K39" s="55">
+        <f t="shared" ref="K39:K54" si="49" xml:space="preserve"> A39*$K$38/(n1_N2*R_N2)</f>
+        <v>172.92699999999996</v>
+      </c>
+      <c r="L39" s="55">
+        <f t="shared" ref="L39:L54" si="50" xml:space="preserve"> A39*$L$38/(n1_N2*R_N2)</f>
+        <v>178.88999999999996</v>
+      </c>
+      <c r="M39" s="55">
+        <f t="shared" ref="M39:M54" si="51" xml:space="preserve"> A39*$M$38/(n1_N2*R_N2)</f>
+        <v>184.85299999999998</v>
+      </c>
+      <c r="N39" s="55">
+        <f t="shared" ref="N39:N54" si="52" xml:space="preserve"> A39*$N$38/(n1_N2*R_N2)</f>
+        <v>190.81599999999997</v>
+      </c>
+      <c r="O39" s="55">
+        <f t="shared" ref="O39:O54" si="53" xml:space="preserve"> A39*$O$38/(n1_N2*R_N2)</f>
+        <v>196.77899999999997</v>
+      </c>
+      <c r="P39" s="55">
+        <f t="shared" ref="P39:P54" si="54" xml:space="preserve"> A39*$P$38/(n1_N2*R_N2)</f>
+        <v>202.74199999999996</v>
+      </c>
+      <c r="Q39" s="55">
+        <f t="shared" ref="Q39:Q54" si="55" xml:space="preserve"> A39*$Q$38/(n1_N2*R_N2)</f>
+        <v>208.70499999999996</v>
+      </c>
+      <c r="R39" s="55">
+        <f t="shared" ref="R39:R54" si="56" xml:space="preserve"> A39*$R$38/(n1_N2*R_N2)</f>
+        <v>214.66799999999995</v>
+      </c>
+      <c r="S39" s="55">
+        <f t="shared" ref="S39:S54" si="57" xml:space="preserve"> A39*$S$38/(n1_N2*R_N2)</f>
+        <v>220.63099999999997</v>
+      </c>
+      <c r="T39" s="55">
+        <f t="shared" ref="T39:T54" si="58" xml:space="preserve"> A39*$T$38/(n1_N2*R_N2)</f>
+        <v>226.59399999999997</v>
+      </c>
+      <c r="U39" s="55">
+        <f t="shared" ref="U39:U54" si="59" xml:space="preserve"> A39*$U$38/(n1_N2*R_N2)</f>
+        <v>232.55699999999996</v>
+      </c>
+      <c r="V39" s="55">
+        <f t="shared" ref="V39:V54" si="60" xml:space="preserve"> A39*$V$38/(n1_N2*R_N2)</f>
+        <v>238.51999999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A40" s="57">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B40" s="55">
+        <f t="shared" si="40"/>
+        <v>131.18599999999998</v>
+      </c>
+      <c r="C40" s="55">
+        <f t="shared" si="41"/>
+        <v>137.74529999999999</v>
+      </c>
+      <c r="D40" s="55">
+        <f t="shared" si="42"/>
+        <v>144.30459999999997</v>
+      </c>
+      <c r="E40" s="55">
+        <f t="shared" si="43"/>
+        <v>150.86389999999997</v>
+      </c>
+      <c r="F40" s="55">
+        <f t="shared" si="44"/>
+        <v>157.42319999999998</v>
+      </c>
+      <c r="G40" s="55">
+        <f t="shared" si="45"/>
+        <v>163.98249999999996</v>
+      </c>
+      <c r="H40" s="55">
+        <f t="shared" si="46"/>
+        <v>170.54179999999999</v>
+      </c>
+      <c r="I40" s="55">
+        <f t="shared" si="47"/>
+        <v>177.1011</v>
+      </c>
+      <c r="J40" s="55">
+        <f t="shared" si="48"/>
+        <v>183.66039999999998</v>
+      </c>
+      <c r="K40" s="55">
+        <f t="shared" si="49"/>
+        <v>190.21969999999999</v>
+      </c>
+      <c r="L40" s="55">
+        <f t="shared" si="50"/>
+        <v>196.779</v>
+      </c>
+      <c r="M40" s="55">
+        <f t="shared" si="51"/>
+        <v>203.3383</v>
+      </c>
+      <c r="N40" s="55">
+        <f t="shared" si="52"/>
+        <v>209.89759999999998</v>
+      </c>
+      <c r="O40" s="55">
+        <f t="shared" si="53"/>
+        <v>216.45689999999999</v>
+      </c>
+      <c r="P40" s="55">
+        <f t="shared" si="54"/>
+        <v>223.0162</v>
+      </c>
+      <c r="Q40" s="55">
+        <f t="shared" si="55"/>
+        <v>229.57549999999998</v>
+      </c>
+      <c r="R40" s="55">
+        <f t="shared" si="56"/>
+        <v>236.13479999999998</v>
+      </c>
+      <c r="S40" s="55">
+        <f t="shared" si="57"/>
+        <v>242.69409999999999</v>
+      </c>
+      <c r="T40" s="55">
+        <f t="shared" si="58"/>
+        <v>249.25339999999994</v>
+      </c>
+      <c r="U40" s="55">
+        <f t="shared" si="59"/>
+        <v>255.81269999999995</v>
+      </c>
+      <c r="V40" s="55">
+        <f t="shared" si="60"/>
+        <v>262.37199999999996</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A41" s="56">
+        <v>1.2</v>
+      </c>
+      <c r="B41" s="55">
+        <f t="shared" si="40"/>
+        <v>143.11199999999997</v>
+      </c>
+      <c r="C41" s="55">
+        <f t="shared" si="41"/>
+        <v>150.26759999999999</v>
+      </c>
+      <c r="D41" s="55">
+        <f t="shared" si="42"/>
+        <v>157.42319999999998</v>
+      </c>
+      <c r="E41" s="55">
+        <f t="shared" si="43"/>
+        <v>164.57879999999997</v>
+      </c>
+      <c r="F41" s="55">
+        <f t="shared" si="44"/>
+        <v>171.73439999999997</v>
+      </c>
+      <c r="G41" s="55">
+        <f t="shared" si="45"/>
+        <v>178.88999999999996</v>
+      </c>
+      <c r="H41" s="55">
+        <f t="shared" si="46"/>
+        <v>186.04559999999998</v>
+      </c>
+      <c r="I41" s="55">
+        <f t="shared" si="47"/>
+        <v>193.20119999999997</v>
+      </c>
+      <c r="J41" s="55">
+        <f t="shared" si="48"/>
+        <v>200.35679999999996</v>
+      </c>
+      <c r="K41" s="55">
+        <f t="shared" si="49"/>
+        <v>207.51239999999996</v>
+      </c>
+      <c r="L41" s="55">
+        <f t="shared" si="50"/>
+        <v>214.66799999999995</v>
+      </c>
+      <c r="M41" s="55">
+        <f t="shared" si="51"/>
+        <v>221.82359999999997</v>
+      </c>
+      <c r="N41" s="55">
+        <f t="shared" si="52"/>
+        <v>228.97919999999996</v>
+      </c>
+      <c r="O41" s="55">
+        <f t="shared" si="53"/>
+        <v>236.13479999999996</v>
+      </c>
+      <c r="P41" s="55">
+        <f t="shared" si="54"/>
+        <v>243.29039999999995</v>
+      </c>
+      <c r="Q41" s="55">
+        <f t="shared" si="55"/>
+        <v>250.44599999999997</v>
+      </c>
+      <c r="R41" s="55">
+        <f t="shared" si="56"/>
+        <v>257.60159999999996</v>
+      </c>
+      <c r="S41" s="55">
+        <f t="shared" si="57"/>
+        <v>264.75719999999995</v>
+      </c>
+      <c r="T41" s="55">
+        <f t="shared" si="58"/>
+        <v>271.91279999999995</v>
+      </c>
+      <c r="U41" s="55">
+        <f t="shared" si="59"/>
+        <v>279.06839999999994</v>
+      </c>
+      <c r="V41" s="55">
+        <f t="shared" si="60"/>
+        <v>286.22399999999993</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A42" s="57">
+        <v>1.3</v>
+      </c>
+      <c r="B42" s="55">
+        <f t="shared" si="40"/>
+        <v>155.03799999999998</v>
+      </c>
+      <c r="C42" s="55">
+        <f t="shared" si="41"/>
+        <v>162.78989999999996</v>
+      </c>
+      <c r="D42" s="55">
+        <f t="shared" si="42"/>
+        <v>170.54179999999997</v>
+      </c>
+      <c r="E42" s="55">
+        <f t="shared" si="43"/>
+        <v>178.29369999999997</v>
+      </c>
+      <c r="F42" s="55">
+        <f t="shared" si="44"/>
+        <v>186.04559999999998</v>
+      </c>
+      <c r="G42" s="55">
+        <f t="shared" si="45"/>
+        <v>193.79749999999996</v>
+      </c>
+      <c r="H42" s="55">
+        <f t="shared" si="46"/>
+        <v>201.54939999999996</v>
+      </c>
+      <c r="I42" s="55">
+        <f t="shared" si="47"/>
+        <v>209.30129999999997</v>
+      </c>
+      <c r="J42" s="55">
+        <f t="shared" si="48"/>
+        <v>217.05319999999998</v>
+      </c>
+      <c r="K42" s="55">
+        <f t="shared" si="49"/>
+        <v>224.80509999999995</v>
+      </c>
+      <c r="L42" s="55">
+        <f t="shared" si="50"/>
+        <v>232.55699999999996</v>
+      </c>
+      <c r="M42" s="55">
+        <f t="shared" si="51"/>
+        <v>240.30889999999997</v>
+      </c>
+      <c r="N42" s="55">
+        <f t="shared" si="52"/>
+        <v>248.06079999999994</v>
+      </c>
+      <c r="O42" s="55">
+        <f t="shared" si="53"/>
+        <v>255.81269999999995</v>
+      </c>
+      <c r="P42" s="55">
+        <f t="shared" si="54"/>
+        <v>263.56459999999993</v>
+      </c>
+      <c r="Q42" s="55">
+        <f t="shared" si="55"/>
+        <v>271.31649999999996</v>
+      </c>
+      <c r="R42" s="55">
+        <f t="shared" si="56"/>
+        <v>279.06839999999994</v>
+      </c>
+      <c r="S42" s="55">
+        <f t="shared" si="57"/>
+        <v>286.82029999999997</v>
+      </c>
+      <c r="T42" s="55">
+        <f t="shared" si="58"/>
+        <v>294.57219999999995</v>
+      </c>
+      <c r="U42" s="55">
+        <f t="shared" si="59"/>
+        <v>302.32409999999993</v>
+      </c>
+      <c r="V42" s="55">
+        <f t="shared" si="60"/>
+        <v>310.07599999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A43" s="56">
+        <v>1.4</v>
+      </c>
+      <c r="B43" s="55">
+        <f t="shared" si="40"/>
+        <v>166.96399999999997</v>
+      </c>
+      <c r="C43" s="55">
+        <f t="shared" si="41"/>
+        <v>175.31219999999996</v>
+      </c>
+      <c r="D43" s="55">
+        <f t="shared" si="42"/>
+        <v>183.66039999999998</v>
+      </c>
+      <c r="E43" s="55">
+        <f t="shared" si="43"/>
+        <v>192.00859999999997</v>
+      </c>
+      <c r="F43" s="55">
+        <f t="shared" si="44"/>
+        <v>200.35679999999996</v>
+      </c>
+      <c r="G43" s="55">
+        <f t="shared" si="45"/>
+        <v>208.70499999999996</v>
+      </c>
+      <c r="H43" s="55">
+        <f t="shared" si="46"/>
+        <v>217.05319999999995</v>
+      </c>
+      <c r="I43" s="55">
+        <f t="shared" si="47"/>
+        <v>225.40139999999994</v>
+      </c>
+      <c r="J43" s="55">
+        <f t="shared" si="48"/>
+        <v>233.74959999999993</v>
+      </c>
+      <c r="K43" s="55">
+        <f t="shared" si="49"/>
+        <v>242.09779999999992</v>
+      </c>
+      <c r="L43" s="55">
+        <f t="shared" si="50"/>
+        <v>250.44599999999997</v>
+      </c>
+      <c r="M43" s="55">
+        <f t="shared" si="51"/>
+        <v>258.79419999999993</v>
+      </c>
+      <c r="N43" s="55">
+        <f t="shared" si="52"/>
+        <v>267.14239999999995</v>
+      </c>
+      <c r="O43" s="55">
+        <f t="shared" si="53"/>
+        <v>275.49059999999997</v>
+      </c>
+      <c r="P43" s="55">
+        <f t="shared" si="54"/>
+        <v>283.83879999999994</v>
+      </c>
+      <c r="Q43" s="55">
+        <f t="shared" si="55"/>
+        <v>292.18699999999995</v>
+      </c>
+      <c r="R43" s="55">
+        <f t="shared" si="56"/>
+        <v>300.53519999999997</v>
+      </c>
+      <c r="S43" s="55">
+        <f t="shared" si="57"/>
+        <v>308.88339999999994</v>
+      </c>
+      <c r="T43" s="55">
+        <f t="shared" si="58"/>
+        <v>317.23159999999996</v>
+      </c>
+      <c r="U43" s="55">
+        <f t="shared" si="59"/>
+        <v>325.57979999999992</v>
+      </c>
+      <c r="V43" s="55">
+        <f t="shared" si="60"/>
+        <v>333.92799999999994</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A44" s="57">
+        <v>1.5</v>
+      </c>
+      <c r="B44" s="55">
+        <f t="shared" si="40"/>
+        <v>178.88999999999996</v>
+      </c>
+      <c r="C44" s="55">
+        <f t="shared" si="41"/>
+        <v>187.83449999999996</v>
+      </c>
+      <c r="D44" s="55">
+        <f t="shared" si="42"/>
+        <v>196.77899999999997</v>
+      </c>
+      <c r="E44" s="55">
+        <f t="shared" si="43"/>
+        <v>205.72349999999997</v>
+      </c>
+      <c r="F44" s="55">
+        <f t="shared" si="44"/>
+        <v>214.66799999999995</v>
+      </c>
+      <c r="G44" s="55">
+        <f t="shared" si="45"/>
+        <v>223.61249999999995</v>
+      </c>
+      <c r="H44" s="55">
+        <f t="shared" si="46"/>
+        <v>232.55699999999996</v>
+      </c>
+      <c r="I44" s="55">
+        <f t="shared" si="47"/>
+        <v>241.50149999999996</v>
+      </c>
+      <c r="J44" s="55">
+        <f t="shared" si="48"/>
+        <v>250.44599999999997</v>
+      </c>
+      <c r="K44" s="55">
+        <f t="shared" si="49"/>
+        <v>259.39049999999997</v>
+      </c>
+      <c r="L44" s="55">
+        <f t="shared" si="50"/>
+        <v>268.33499999999998</v>
+      </c>
+      <c r="M44" s="55">
+        <f t="shared" si="51"/>
+        <v>277.27949999999993</v>
+      </c>
+      <c r="N44" s="55">
+        <f t="shared" si="52"/>
+        <v>286.22399999999993</v>
+      </c>
+      <c r="O44" s="55">
+        <f t="shared" si="53"/>
+        <v>295.16849999999994</v>
+      </c>
+      <c r="P44" s="55">
+        <f t="shared" si="54"/>
+        <v>304.11299999999994</v>
+      </c>
+      <c r="Q44" s="55">
+        <f t="shared" si="55"/>
+        <v>313.05749999999995</v>
+      </c>
+      <c r="R44" s="55">
+        <f t="shared" si="56"/>
+        <v>322.00199999999995</v>
+      </c>
+      <c r="S44" s="55">
+        <f t="shared" si="57"/>
+        <v>330.94649999999996</v>
+      </c>
+      <c r="T44" s="55">
+        <f t="shared" si="58"/>
+        <v>339.89099999999996</v>
+      </c>
+      <c r="U44" s="55">
+        <f t="shared" si="59"/>
+        <v>348.83549999999991</v>
+      </c>
+      <c r="V44" s="55">
+        <f t="shared" si="60"/>
+        <v>357.77999999999992</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A45" s="56">
+        <v>1.6</v>
+      </c>
+      <c r="B45" s="55">
+        <f t="shared" si="40"/>
+        <v>190.81599999999997</v>
+      </c>
+      <c r="C45" s="55">
+        <f t="shared" si="41"/>
+        <v>200.35679999999996</v>
+      </c>
+      <c r="D45" s="55">
+        <f t="shared" si="42"/>
+        <v>209.89759999999995</v>
+      </c>
+      <c r="E45" s="55">
+        <f t="shared" si="43"/>
+        <v>219.43839999999997</v>
+      </c>
+      <c r="F45" s="55">
+        <f t="shared" si="44"/>
+        <v>228.97919999999996</v>
+      </c>
+      <c r="G45" s="55">
+        <f t="shared" si="45"/>
+        <v>238.51999999999995</v>
+      </c>
+      <c r="H45" s="55">
+        <f t="shared" si="46"/>
+        <v>248.06079999999994</v>
+      </c>
+      <c r="I45" s="55">
+        <f t="shared" si="47"/>
+        <v>257.60159999999996</v>
+      </c>
+      <c r="J45" s="55">
+        <f t="shared" si="48"/>
+        <v>267.14239999999995</v>
+      </c>
+      <c r="K45" s="55">
+        <f t="shared" si="49"/>
+        <v>276.68319999999994</v>
+      </c>
+      <c r="L45" s="55">
+        <f t="shared" si="50"/>
+        <v>286.22399999999993</v>
+      </c>
+      <c r="M45" s="55">
+        <f t="shared" si="51"/>
+        <v>295.76479999999992</v>
+      </c>
+      <c r="N45" s="55">
+        <f t="shared" si="52"/>
+        <v>305.30559999999997</v>
+      </c>
+      <c r="O45" s="55">
+        <f t="shared" si="53"/>
+        <v>314.84639999999996</v>
+      </c>
+      <c r="P45" s="55">
+        <f t="shared" si="54"/>
+        <v>324.38719999999995</v>
+      </c>
+      <c r="Q45" s="55">
+        <f t="shared" si="55"/>
+        <v>333.92799999999994</v>
+      </c>
+      <c r="R45" s="55">
+        <f t="shared" si="56"/>
+        <v>343.46879999999993</v>
+      </c>
+      <c r="S45" s="55">
+        <f t="shared" si="57"/>
+        <v>353.00959999999992</v>
+      </c>
+      <c r="T45" s="55">
+        <f t="shared" si="58"/>
+        <v>362.55039999999991</v>
+      </c>
+      <c r="U45" s="55">
+        <f t="shared" si="59"/>
+        <v>372.09119999999996</v>
+      </c>
+      <c r="V45" s="55">
+        <f t="shared" si="60"/>
+        <v>381.63199999999995</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A46" s="57">
+        <v>1.7</v>
+      </c>
+      <c r="B46" s="55">
+        <f t="shared" si="40"/>
+        <v>202.74199999999996</v>
+      </c>
+      <c r="C46" s="55">
+        <f t="shared" si="41"/>
+        <v>212.87909999999997</v>
+      </c>
+      <c r="D46" s="55">
+        <f t="shared" si="42"/>
+        <v>223.01619999999997</v>
+      </c>
+      <c r="E46" s="55">
+        <f t="shared" si="43"/>
+        <v>233.15329999999997</v>
+      </c>
+      <c r="F46" s="55">
+        <f t="shared" si="44"/>
+        <v>243.29039999999995</v>
+      </c>
+      <c r="G46" s="55">
+        <f t="shared" si="45"/>
+        <v>253.42749999999995</v>
+      </c>
+      <c r="H46" s="55">
+        <f t="shared" si="46"/>
+        <v>263.56459999999993</v>
+      </c>
+      <c r="I46" s="55">
+        <f t="shared" si="47"/>
+        <v>273.70169999999996</v>
+      </c>
+      <c r="J46" s="55">
+        <f t="shared" si="48"/>
+        <v>283.83879999999994</v>
+      </c>
+      <c r="K46" s="55">
+        <f t="shared" si="49"/>
+        <v>293.97589999999997</v>
+      </c>
+      <c r="L46" s="55">
+        <f t="shared" si="50"/>
+        <v>304.11299999999994</v>
+      </c>
+      <c r="M46" s="55">
+        <f t="shared" si="51"/>
+        <v>314.25009999999992</v>
+      </c>
+      <c r="N46" s="55">
+        <f t="shared" si="52"/>
+        <v>324.38719999999995</v>
+      </c>
+      <c r="O46" s="55">
+        <f t="shared" si="53"/>
+        <v>334.52429999999993</v>
+      </c>
+      <c r="P46" s="55">
+        <f t="shared" si="54"/>
+        <v>344.66139999999996</v>
+      </c>
+      <c r="Q46" s="55">
+        <f t="shared" si="55"/>
+        <v>354.79849999999993</v>
+      </c>
+      <c r="R46" s="55">
+        <f t="shared" si="56"/>
+        <v>364.93559999999991</v>
+      </c>
+      <c r="S46" s="55">
+        <f t="shared" si="57"/>
+        <v>375.07269999999994</v>
+      </c>
+      <c r="T46" s="55">
+        <f t="shared" si="58"/>
+        <v>385.20979999999992</v>
+      </c>
+      <c r="U46" s="55">
+        <f t="shared" si="59"/>
+        <v>395.34689999999995</v>
+      </c>
+      <c r="V46" s="55">
+        <f t="shared" si="60"/>
+        <v>405.48399999999992</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A47" s="56">
+        <v>1.8</v>
+      </c>
+      <c r="B47" s="55">
+        <f t="shared" si="40"/>
+        <v>214.66799999999995</v>
+      </c>
+      <c r="C47" s="55">
+        <f t="shared" si="41"/>
+        <v>225.40139999999997</v>
+      </c>
+      <c r="D47" s="55">
+        <f t="shared" si="42"/>
+        <v>236.13479999999996</v>
+      </c>
+      <c r="E47" s="55">
+        <f t="shared" si="43"/>
+        <v>246.86819999999994</v>
+      </c>
+      <c r="F47" s="55">
+        <f t="shared" si="44"/>
+        <v>257.60159999999996</v>
+      </c>
+      <c r="G47" s="55">
+        <f t="shared" si="45"/>
+        <v>268.33499999999998</v>
+      </c>
+      <c r="H47" s="55">
+        <f t="shared" si="46"/>
+        <v>279.06839999999994</v>
+      </c>
+      <c r="I47" s="55">
+        <f t="shared" si="47"/>
+        <v>289.80179999999996</v>
+      </c>
+      <c r="J47" s="55">
+        <f t="shared" si="48"/>
+        <v>300.53519999999997</v>
+      </c>
+      <c r="K47" s="55">
+        <f t="shared" si="49"/>
+        <v>311.26859999999994</v>
+      </c>
+      <c r="L47" s="55">
+        <f t="shared" si="50"/>
+        <v>322.00199999999995</v>
+      </c>
+      <c r="M47" s="55">
+        <f t="shared" si="51"/>
+        <v>332.73539999999991</v>
+      </c>
+      <c r="N47" s="55">
+        <f t="shared" si="52"/>
+        <v>343.46879999999993</v>
+      </c>
+      <c r="O47" s="55">
+        <f t="shared" si="53"/>
+        <v>354.20219999999995</v>
+      </c>
+      <c r="P47" s="55">
+        <f t="shared" si="54"/>
+        <v>364.93559999999991</v>
+      </c>
+      <c r="Q47" s="55">
+        <f t="shared" si="55"/>
+        <v>375.66899999999993</v>
+      </c>
+      <c r="R47" s="55">
+        <f t="shared" si="56"/>
+        <v>386.40239999999994</v>
+      </c>
+      <c r="S47" s="55">
+        <f t="shared" si="57"/>
+        <v>397.1357999999999</v>
+      </c>
+      <c r="T47" s="55">
+        <f t="shared" si="58"/>
+        <v>407.86919999999992</v>
+      </c>
+      <c r="U47" s="55">
+        <f t="shared" si="59"/>
+        <v>418.60259999999994</v>
+      </c>
+      <c r="V47" s="55">
+        <f t="shared" si="60"/>
+        <v>429.3359999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A48" s="57">
+        <v>1.9</v>
+      </c>
+      <c r="B48" s="55">
+        <f t="shared" si="40"/>
+        <v>226.59399999999997</v>
+      </c>
+      <c r="C48" s="55">
+        <f t="shared" si="41"/>
+        <v>237.92369999999997</v>
+      </c>
+      <c r="D48" s="55">
+        <f t="shared" si="42"/>
+        <v>249.25339999999994</v>
+      </c>
+      <c r="E48" s="55">
+        <f t="shared" si="43"/>
+        <v>260.58309999999994</v>
+      </c>
+      <c r="F48" s="55">
+        <f t="shared" si="44"/>
+        <v>271.91279999999995</v>
+      </c>
+      <c r="G48" s="55">
+        <f t="shared" si="45"/>
+        <v>283.24249999999995</v>
+      </c>
+      <c r="H48" s="55">
+        <f t="shared" si="46"/>
+        <v>294.57219999999995</v>
+      </c>
+      <c r="I48" s="55">
+        <f t="shared" si="47"/>
+        <v>305.90189999999996</v>
+      </c>
+      <c r="J48" s="55">
+        <f t="shared" si="48"/>
+        <v>317.23159999999996</v>
+      </c>
+      <c r="K48" s="55">
+        <f t="shared" si="49"/>
+        <v>328.56129999999996</v>
+      </c>
+      <c r="L48" s="55">
+        <f t="shared" si="50"/>
+        <v>339.89099999999996</v>
+      </c>
+      <c r="M48" s="55">
+        <f t="shared" si="51"/>
+        <v>351.22069999999997</v>
+      </c>
+      <c r="N48" s="55">
+        <f t="shared" si="52"/>
+        <v>362.55039999999991</v>
+      </c>
+      <c r="O48" s="55">
+        <f t="shared" si="53"/>
+        <v>373.88009999999991</v>
+      </c>
+      <c r="P48" s="55">
+        <f t="shared" si="54"/>
+        <v>385.20979999999992</v>
+      </c>
+      <c r="Q48" s="55">
+        <f t="shared" si="55"/>
+        <v>396.53949999999992</v>
+      </c>
+      <c r="R48" s="55">
+        <f t="shared" si="56"/>
+        <v>407.86919999999992</v>
+      </c>
+      <c r="S48" s="55">
+        <f t="shared" si="57"/>
+        <v>419.19889999999992</v>
+      </c>
+      <c r="T48" s="55">
+        <f t="shared" si="58"/>
+        <v>430.52859999999993</v>
+      </c>
+      <c r="U48" s="55">
+        <f t="shared" si="59"/>
+        <v>441.85829999999993</v>
+      </c>
+      <c r="V48" s="55">
+        <f t="shared" si="60"/>
+        <v>453.18799999999993</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A49" s="56">
+        <v>2</v>
+      </c>
+      <c r="B49" s="55">
+        <f t="shared" si="40"/>
+        <v>238.51999999999995</v>
+      </c>
+      <c r="C49" s="55">
+        <f t="shared" si="41"/>
+        <v>250.44599999999997</v>
+      </c>
+      <c r="D49" s="55">
+        <f t="shared" si="42"/>
+        <v>262.37199999999996</v>
+      </c>
+      <c r="E49" s="55">
+        <f t="shared" si="43"/>
+        <v>274.29799999999994</v>
+      </c>
+      <c r="F49" s="55">
+        <f t="shared" si="44"/>
+        <v>286.22399999999993</v>
+      </c>
+      <c r="G49" s="55">
+        <f t="shared" si="45"/>
+        <v>298.14999999999992</v>
+      </c>
+      <c r="H49" s="55">
+        <f t="shared" si="46"/>
+        <v>310.07599999999996</v>
+      </c>
+      <c r="I49" s="55">
+        <f t="shared" si="47"/>
+        <v>322.00199999999995</v>
+      </c>
+      <c r="J49" s="55">
+        <f t="shared" si="48"/>
+        <v>333.92799999999994</v>
+      </c>
+      <c r="K49" s="55">
+        <f t="shared" si="49"/>
+        <v>345.85399999999993</v>
+      </c>
+      <c r="L49" s="55">
+        <f t="shared" si="50"/>
+        <v>357.77999999999992</v>
+      </c>
+      <c r="M49" s="55">
+        <f t="shared" si="51"/>
+        <v>369.70599999999996</v>
+      </c>
+      <c r="N49" s="55">
+        <f t="shared" si="52"/>
+        <v>381.63199999999995</v>
+      </c>
+      <c r="O49" s="55">
+        <f t="shared" si="53"/>
+        <v>393.55799999999994</v>
+      </c>
+      <c r="P49" s="55">
+        <f t="shared" si="54"/>
+        <v>405.48399999999992</v>
+      </c>
+      <c r="Q49" s="55">
+        <f t="shared" si="55"/>
+        <v>417.40999999999991</v>
+      </c>
+      <c r="R49" s="55">
+        <f t="shared" si="56"/>
+        <v>429.3359999999999</v>
+      </c>
+      <c r="S49" s="55">
+        <f t="shared" si="57"/>
+        <v>441.26199999999994</v>
+      </c>
+      <c r="T49" s="55">
+        <f t="shared" si="58"/>
+        <v>453.18799999999993</v>
+      </c>
+      <c r="U49" s="55">
+        <f t="shared" si="59"/>
+        <v>465.11399999999992</v>
+      </c>
+      <c r="V49" s="55">
+        <f t="shared" si="60"/>
+        <v>477.03999999999991</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A50" s="57">
+        <v>2.1</v>
+      </c>
+      <c r="B50" s="55">
+        <f t="shared" si="40"/>
+        <v>250.44599999999997</v>
+      </c>
+      <c r="C50" s="55">
+        <f t="shared" si="41"/>
+        <v>262.96829999999994</v>
+      </c>
+      <c r="D50" s="55">
+        <f t="shared" si="42"/>
+        <v>275.49059999999997</v>
+      </c>
+      <c r="E50" s="55">
+        <f t="shared" si="43"/>
+        <v>288.01289999999995</v>
+      </c>
+      <c r="F50" s="55">
+        <f t="shared" si="44"/>
+        <v>300.53519999999997</v>
+      </c>
+      <c r="G50" s="55">
+        <f t="shared" si="45"/>
+        <v>313.05749999999995</v>
+      </c>
+      <c r="H50" s="55">
+        <f t="shared" si="46"/>
+        <v>325.57979999999992</v>
+      </c>
+      <c r="I50" s="55">
+        <f t="shared" si="47"/>
+        <v>338.10209999999995</v>
+      </c>
+      <c r="J50" s="55">
+        <f t="shared" si="48"/>
+        <v>350.62439999999992</v>
+      </c>
+      <c r="K50" s="55">
+        <f t="shared" si="49"/>
+        <v>363.14669999999995</v>
+      </c>
+      <c r="L50" s="55">
+        <f t="shared" si="50"/>
+        <v>375.66899999999993</v>
+      </c>
+      <c r="M50" s="55">
+        <f t="shared" si="51"/>
+        <v>388.19129999999996</v>
+      </c>
+      <c r="N50" s="55">
+        <f t="shared" si="52"/>
+        <v>400.71359999999993</v>
+      </c>
+      <c r="O50" s="55">
+        <f t="shared" si="53"/>
+        <v>413.2358999999999</v>
+      </c>
+      <c r="P50" s="55">
+        <f t="shared" si="54"/>
+        <v>425.75819999999993</v>
+      </c>
+      <c r="Q50" s="55">
+        <f t="shared" si="55"/>
+        <v>438.2804999999999</v>
+      </c>
+      <c r="R50" s="55">
+        <f t="shared" si="56"/>
+        <v>450.80279999999993</v>
+      </c>
+      <c r="S50" s="55">
+        <f t="shared" si="57"/>
+        <v>463.32509999999991</v>
+      </c>
+      <c r="T50" s="55">
+        <f t="shared" si="58"/>
+        <v>475.84739999999994</v>
+      </c>
+      <c r="U50" s="55">
+        <f t="shared" si="59"/>
+        <v>488.36969999999991</v>
+      </c>
+      <c r="V50" s="55">
+        <f t="shared" si="60"/>
+        <v>500.89199999999994</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A51" s="56">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B51" s="55">
+        <f t="shared" si="40"/>
+        <v>262.37199999999996</v>
+      </c>
+      <c r="C51" s="55">
+        <f t="shared" si="41"/>
+        <v>275.49059999999997</v>
+      </c>
+      <c r="D51" s="55">
+        <f t="shared" si="42"/>
+        <v>288.60919999999993</v>
+      </c>
+      <c r="E51" s="55">
+        <f t="shared" si="43"/>
+        <v>301.72779999999995</v>
+      </c>
+      <c r="F51" s="55">
+        <f t="shared" si="44"/>
+        <v>314.84639999999996</v>
+      </c>
+      <c r="G51" s="55">
+        <f t="shared" si="45"/>
+        <v>327.96499999999992</v>
+      </c>
+      <c r="H51" s="55">
+        <f t="shared" si="46"/>
+        <v>341.08359999999999</v>
+      </c>
+      <c r="I51" s="55">
+        <f t="shared" si="47"/>
+        <v>354.2022</v>
+      </c>
+      <c r="J51" s="55">
+        <f t="shared" si="48"/>
+        <v>367.32079999999996</v>
+      </c>
+      <c r="K51" s="55">
+        <f t="shared" si="49"/>
+        <v>380.43939999999998</v>
+      </c>
+      <c r="L51" s="55">
+        <f t="shared" si="50"/>
+        <v>393.55799999999999</v>
+      </c>
+      <c r="M51" s="55">
+        <f t="shared" si="51"/>
+        <v>406.67660000000001</v>
+      </c>
+      <c r="N51" s="55">
+        <f t="shared" si="52"/>
+        <v>419.79519999999997</v>
+      </c>
+      <c r="O51" s="55">
+        <f t="shared" si="53"/>
+        <v>432.91379999999998</v>
+      </c>
+      <c r="P51" s="55">
+        <f t="shared" si="54"/>
+        <v>446.0324</v>
+      </c>
+      <c r="Q51" s="55">
+        <f t="shared" si="55"/>
+        <v>459.15099999999995</v>
+      </c>
+      <c r="R51" s="55">
+        <f t="shared" si="56"/>
+        <v>472.26959999999997</v>
+      </c>
+      <c r="S51" s="55">
+        <f t="shared" si="57"/>
+        <v>485.38819999999998</v>
+      </c>
+      <c r="T51" s="55">
+        <f t="shared" si="58"/>
+        <v>498.50679999999988</v>
+      </c>
+      <c r="U51" s="55">
+        <f t="shared" si="59"/>
+        <v>511.6253999999999</v>
+      </c>
+      <c r="V51" s="55">
+        <f t="shared" si="60"/>
+        <v>524.74399999999991</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A52" s="57">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B52" s="55">
+        <f t="shared" si="40"/>
+        <v>274.29799999999994</v>
+      </c>
+      <c r="C52" s="55">
+        <f t="shared" si="41"/>
+        <v>288.01289999999995</v>
+      </c>
+      <c r="D52" s="55">
+        <f t="shared" si="42"/>
+        <v>301.72779999999995</v>
+      </c>
+      <c r="E52" s="55">
+        <f t="shared" si="43"/>
+        <v>315.44269999999995</v>
+      </c>
+      <c r="F52" s="55">
+        <f t="shared" si="44"/>
+        <v>329.15759999999995</v>
+      </c>
+      <c r="G52" s="55">
+        <f t="shared" si="45"/>
+        <v>342.87249999999995</v>
+      </c>
+      <c r="H52" s="55">
+        <f t="shared" si="46"/>
+        <v>356.58739999999989</v>
+      </c>
+      <c r="I52" s="55">
+        <f t="shared" si="47"/>
+        <v>370.30229999999989</v>
+      </c>
+      <c r="J52" s="55">
+        <f t="shared" si="48"/>
+        <v>384.01719999999989</v>
+      </c>
+      <c r="K52" s="55">
+        <f t="shared" si="49"/>
+        <v>397.73209999999989</v>
+      </c>
+      <c r="L52" s="55">
+        <f t="shared" si="50"/>
+        <v>411.44699999999989</v>
+      </c>
+      <c r="M52" s="55">
+        <f t="shared" si="51"/>
+        <v>425.16189999999989</v>
+      </c>
+      <c r="N52" s="55">
+        <f t="shared" si="52"/>
+        <v>438.87679999999989</v>
+      </c>
+      <c r="O52" s="55">
+        <f t="shared" si="53"/>
+        <v>452.59169999999989</v>
+      </c>
+      <c r="P52" s="55">
+        <f t="shared" si="54"/>
+        <v>466.30659999999989</v>
+      </c>
+      <c r="Q52" s="55">
+        <f t="shared" si="55"/>
+        <v>480.02149999999989</v>
+      </c>
+      <c r="R52" s="55">
+        <f t="shared" si="56"/>
+        <v>493.73639999999989</v>
+      </c>
+      <c r="S52" s="55">
+        <f t="shared" si="57"/>
+        <v>507.45129999999989</v>
+      </c>
+      <c r="T52" s="55">
+        <f t="shared" si="58"/>
+        <v>521.16619999999989</v>
+      </c>
+      <c r="U52" s="55">
+        <f t="shared" si="59"/>
+        <v>534.88109999999995</v>
+      </c>
+      <c r="V52" s="55">
+        <f t="shared" si="60"/>
+        <v>548.59599999999989</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A53" s="56">
+        <v>2.4</v>
+      </c>
+      <c r="B53" s="55">
+        <f t="shared" si="40"/>
+        <v>286.22399999999993</v>
+      </c>
+      <c r="C53" s="55">
+        <f t="shared" si="41"/>
+        <v>300.53519999999997</v>
+      </c>
+      <c r="D53" s="55">
+        <f t="shared" si="42"/>
+        <v>314.84639999999996</v>
+      </c>
+      <c r="E53" s="55">
+        <f t="shared" si="43"/>
+        <v>329.15759999999995</v>
+      </c>
+      <c r="F53" s="55">
+        <f t="shared" si="44"/>
+        <v>343.46879999999993</v>
+      </c>
+      <c r="G53" s="55">
+        <f t="shared" si="45"/>
+        <v>357.77999999999992</v>
+      </c>
+      <c r="H53" s="55">
+        <f t="shared" si="46"/>
+        <v>372.09119999999996</v>
+      </c>
+      <c r="I53" s="55">
+        <f t="shared" si="47"/>
+        <v>386.40239999999994</v>
+      </c>
+      <c r="J53" s="55">
+        <f t="shared" si="48"/>
+        <v>400.71359999999993</v>
+      </c>
+      <c r="K53" s="55">
+        <f t="shared" si="49"/>
+        <v>415.02479999999991</v>
+      </c>
+      <c r="L53" s="55">
+        <f t="shared" si="50"/>
+        <v>429.3359999999999</v>
+      </c>
+      <c r="M53" s="55">
+        <f t="shared" si="51"/>
+        <v>443.64719999999994</v>
+      </c>
+      <c r="N53" s="55">
+        <f t="shared" si="52"/>
+        <v>457.95839999999993</v>
+      </c>
+      <c r="O53" s="55">
+        <f t="shared" si="53"/>
+        <v>472.26959999999991</v>
+      </c>
+      <c r="P53" s="55">
+        <f t="shared" si="54"/>
+        <v>486.5807999999999</v>
+      </c>
+      <c r="Q53" s="55">
+        <f t="shared" si="55"/>
+        <v>500.89199999999994</v>
+      </c>
+      <c r="R53" s="55">
+        <f t="shared" si="56"/>
+        <v>515.20319999999992</v>
+      </c>
+      <c r="S53" s="55">
+        <f t="shared" si="57"/>
+        <v>529.51439999999991</v>
+      </c>
+      <c r="T53" s="55">
+        <f t="shared" si="58"/>
+        <v>543.82559999999989</v>
+      </c>
+      <c r="U53" s="55">
+        <f t="shared" si="59"/>
+        <v>558.13679999999988</v>
+      </c>
+      <c r="V53" s="55">
+        <f t="shared" si="60"/>
+        <v>572.44799999999987</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A54" s="57">
+        <v>2.5</v>
+      </c>
+      <c r="B54" s="55">
+        <f t="shared" si="40"/>
+        <v>298.14999999999992</v>
+      </c>
+      <c r="C54" s="55">
+        <f t="shared" si="41"/>
+        <v>313.05749999999995</v>
+      </c>
+      <c r="D54" s="55">
+        <f t="shared" si="42"/>
+        <v>327.96499999999992</v>
+      </c>
+      <c r="E54" s="55">
+        <f t="shared" si="43"/>
+        <v>342.87249999999995</v>
+      </c>
+      <c r="F54" s="55">
+        <f t="shared" si="44"/>
+        <v>357.77999999999992</v>
+      </c>
+      <c r="G54" s="55">
+        <f t="shared" si="45"/>
+        <v>372.68749999999994</v>
+      </c>
+      <c r="H54" s="55">
+        <f t="shared" si="46"/>
+        <v>387.59499999999991</v>
+      </c>
+      <c r="I54" s="55">
+        <f t="shared" si="47"/>
+        <v>402.50249999999994</v>
+      </c>
+      <c r="J54" s="55">
+        <f t="shared" si="48"/>
+        <v>417.40999999999991</v>
+      </c>
+      <c r="K54" s="55">
+        <f t="shared" si="49"/>
+        <v>432.31749999999994</v>
+      </c>
+      <c r="L54" s="55">
+        <f t="shared" si="50"/>
+        <v>447.22499999999991</v>
+      </c>
+      <c r="M54" s="55">
+        <f t="shared" si="51"/>
+        <v>462.13249999999994</v>
+      </c>
+      <c r="N54" s="55">
+        <f t="shared" si="52"/>
+        <v>477.03999999999991</v>
+      </c>
+      <c r="O54" s="55">
+        <f t="shared" si="53"/>
+        <v>491.94749999999993</v>
+      </c>
+      <c r="P54" s="55">
+        <f t="shared" si="54"/>
+        <v>506.8549999999999</v>
+      </c>
+      <c r="Q54" s="55">
+        <f t="shared" si="55"/>
+        <v>521.76249999999993</v>
+      </c>
+      <c r="R54" s="55">
+        <f t="shared" si="56"/>
+        <v>536.66999999999996</v>
+      </c>
+      <c r="S54" s="55">
+        <f t="shared" si="57"/>
+        <v>551.57749999999987</v>
+      </c>
+      <c r="T54" s="55">
+        <f t="shared" si="58"/>
+        <v>566.4849999999999</v>
+      </c>
+      <c r="U54" s="55">
+        <f t="shared" si="59"/>
+        <v>581.39249999999993</v>
+      </c>
+      <c r="V54" s="55">
+        <f t="shared" si="60"/>
+        <v>596.29999999999984</v>
       </c>
     </row>
   </sheetData>
@@ -25398,7 +26881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D919DEE-0E37-4D8A-B84D-02339E95CCB3}">
   <dimension ref="B3:T101"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="25" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView zoomScale="25" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="AO72" sqref="AO72"/>
     </sheetView>
   </sheetViews>
@@ -29828,7 +31311,7 @@
   <dimension ref="B1:J33"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScale="33" workbookViewId="0">
-      <selection activeCell="W84" sqref="W84"/>
+      <selection activeCell="AU47" sqref="AU47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34972,7 +36455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275DC24D-743A-4D82-8E81-9D35E9C95C24}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="96" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>

</xml_diff>